<commit_message>
fixed guest name issue for compare_booking
</commit_message>
<xml_diff>
--- a/working_windows_extension/version_3/booking/dist/Customers Not found.xlsx
+++ b/working_windows_extension/version_3/booking/dist/Customers Not found.xlsx
@@ -14,114 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>IBRAHIM ETHEM GECIM</t>
+    <t>Fabiana Santos de Almeida</t>
   </si>
   <si>
-    <t>jianheng wu; wu jianheng</t>
+    <t>Axel Staudenmayer</t>
   </si>
   <si>
-    <t>Tanajah  Green</t>
-  </si>
-  <si>
-    <t>Doreen  Young</t>
-  </si>
-  <si>
-    <t>Deja  Stanley</t>
-  </si>
-  <si>
-    <t>Kristian Toven Diesen; Rolf Diesen, Ellen Louise Toven Diesen</t>
-  </si>
-  <si>
-    <t>Khanh  Nguyen</t>
-  </si>
-  <si>
-    <t>Marvin  von Fintel</t>
-  </si>
-  <si>
-    <t>Monique  Thaxter</t>
-  </si>
-  <si>
-    <t>Alvaro Javier Correa Fernandez</t>
-  </si>
-  <si>
-    <t>KayLee  Taylor</t>
-  </si>
-  <si>
-    <t>Maurice  Baldwin</t>
-  </si>
-  <si>
-    <t>Angela Kerwin</t>
-  </si>
-  <si>
-    <t>Charles  Brown</t>
-  </si>
-  <si>
-    <t>Haiying Wang; Xuhong Guo; Yongsheng Li</t>
-  </si>
-  <si>
-    <t>TimothyJoseph  Dunham</t>
-  </si>
-  <si>
-    <t>María Jesús Reguillo García</t>
-  </si>
-  <si>
-    <t>黄 龙</t>
-  </si>
-  <si>
-    <t>Claudio  ALVAREZ</t>
-  </si>
-  <si>
-    <t>Ivan Dalia; Julio R Narciso; Liz Jara Caballero</t>
-  </si>
-  <si>
-    <t>Sandra Radulović</t>
-  </si>
-  <si>
-    <t>Katie Richard</t>
-  </si>
-  <si>
-    <t>Juan Carlos Cornejo Castro</t>
-  </si>
-  <si>
-    <t>Cyndi Kirby; Hank Gogloza</t>
-  </si>
-  <si>
-    <t>Christopher Grosswiler</t>
-  </si>
-  <si>
-    <t>cynthia grenzebach</t>
-  </si>
-  <si>
-    <t>Caroline Costamilan</t>
-  </si>
-  <si>
-    <t>ZIFEI, ZHAO</t>
-  </si>
-  <si>
-    <t>Gaëlle VINCENT</t>
-  </si>
-  <si>
-    <t>William  Freeman</t>
-  </si>
-  <si>
-    <t>cristina esquivel; omar bedascarrasbure</t>
-  </si>
-  <si>
-    <t>Alysia  Clarke</t>
-  </si>
-  <si>
-    <t>Eva Christine Schitter</t>
-  </si>
-  <si>
-    <t>Romana Cihlářová</t>
-  </si>
-  <si>
-    <t>Robbie  Villacampa</t>
-  </si>
-  <si>
-    <t>Hunter  Wuensche</t>
+    <t>monica judith de la peña toledo</t>
   </si>
 </sst>
 </file>
@@ -453,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,176 +375,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>